<commit_message>
Completed update to 1st iteration coding and data
</commit_message>
<xml_diff>
--- a/data/data for tables/intervention_table.xlsx
+++ b/data/data for tables/intervention_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9748fb32d9e42f0/Desktop/Galenos/LS2/Datafor 1st update and 1st iteration/data for analysis. LSR2 1st iteration new/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9748fb32d9e42f0/Desktop/Github rep/LSR2_exercise_H/data/data for tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_EF6FFDCE8F79A8D366075C52F3A592314597F6DA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D204393-5A31-4B02-9F60-1A5EE8B51339}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_EF6FFDCE8F79A8D366075C52F3A592314597F6DA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0918930D-9644-4627-9E7B-D7CFD92E4532}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,7 +605,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>

</xml_diff>